<commit_message>
reactorizando codigos y agregando logica de deteccion de errores
</commit_message>
<xml_diff>
--- a/SRC/Notas_Alumnos.xlsx
+++ b/SRC/Notas_Alumnos.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20371"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F7122F-376E-48F0-A7F3-43DD24576880}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Notas" sheetId="1" r:id="rId1"/>
@@ -14,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Notas!$A$1:$E$31</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -182,7 +181,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -541,19 +540,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E363"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -570,7 +571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -587,7 +588,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -604,7 +605,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -621,7 +622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -638,7 +639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -655,7 +656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -672,7 +673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -689,7 +690,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -706,7 +707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -723,7 +724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -740,7 +741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -757,7 +758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -774,7 +775,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -791,7 +792,7 @@
         <v>9.796413303830354</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -805,10 +806,10 @@
         <v>10</v>
       </c>
       <c r="E15" s="3">
-        <v>8.9942031394497359</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>8.9942031394497395</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -825,7 +826,7 @@
         <v>8.81864221186847</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -839,10 +840,10 @@
         <v>8.9757090461547744</v>
       </c>
       <c r="E17" s="3">
-        <v>8.4589792455814479</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>8.9942031394497395</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -859,7 +860,7 @@
         <v>8.0993728640911886</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -876,7 +877,7 @@
         <v>9.1659533503359683</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -893,7 +894,7 @@
         <v>8.8712947066397145</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -910,7 +911,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -927,7 +928,7 @@
         <v>8.6082965700161864</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -944,7 +945,7 @@
         <v>9.5921290309149132</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
@@ -961,7 +962,7 @@
         <v>9.4713964525188619</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
@@ -978,7 +979,7 @@
         <v>8.6144376262830225</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
@@ -995,7 +996,7 @@
         <v>9.9642222687372684</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -1006,13 +1007,13 @@
         <v>7.5164794501909959</v>
       </c>
       <c r="D27" s="3">
-        <v>7.289711992972931</v>
+        <v>8.5250000000000004</v>
       </c>
       <c r="E27" s="3">
         <v>7.7492057411030908</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -1029,7 +1030,7 @@
         <v>7.5600701572668729</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
@@ -1046,7 +1047,7 @@
         <v>8.8951636675609507</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
@@ -1063,7 +1064,7 @@
         <v>9.1341825062909514</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
@@ -1080,7 +1081,7 @@
         <v>9.9386266692150063</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -1097,7 +1098,7 @@
         <v>9.1970895986123224</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -1114,7 +1115,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -1131,7 +1132,7 @@
         <v>8.2386507948036147</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
@@ -1148,7 +1149,7 @@
         <v>7.1276368258832097</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>31</v>
       </c>
@@ -1165,7 +1166,7 @@
         <v>8.2547192135805485</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
@@ -1182,7 +1183,7 @@
         <v>8.0603671285744589</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>21</v>
       </c>
@@ -1199,7 +1200,7 @@
         <v>7.7145865087783463</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>21</v>
       </c>
@@ -1216,7 +1217,7 @@
         <v>7.3862881799694646</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>21</v>
       </c>
@@ -1233,7 +1234,7 @@
         <v>7.0331313498533792</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>21</v>
       </c>
@@ -1250,7 +1251,7 @@
         <v>9.8495215609774647</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>21</v>
       </c>
@@ -1267,7 +1268,7 @@
         <v>8.8223751432983484</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>21</v>
       </c>
@@ -1284,7 +1285,7 @@
         <v>7.1326898013260775</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>21</v>
       </c>
@@ -1301,7 +1302,7 @@
         <v>8.1687733180895545</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>21</v>
       </c>
@@ -1318,7 +1319,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>21</v>
       </c>
@@ -1335,7 +1336,7 @@
         <v>7.1535637064901474</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>21</v>
       </c>
@@ -1352,7 +1353,7 @@
         <v>7.1817534204990867</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>21</v>
       </c>
@@ -1369,7 +1370,7 @@
         <v>9.3697867787187796</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>21</v>
       </c>
@@ -1386,7 +1387,7 @@
         <v>7.9178114814171412</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>22</v>
       </c>
@@ -1403,7 +1404,7 @@
         <v>7.725735274458323</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>22</v>
       </c>
@@ -1420,7 +1421,7 @@
         <v>8.5477871618476726</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>22</v>
       </c>
@@ -1437,7 +1438,7 @@
         <v>7.611103034266451</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>22</v>
       </c>
@@ -1454,7 +1455,7 @@
         <v>7.3728608502926045</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>22</v>
       </c>
@@ -1471,7 +1472,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>22</v>
       </c>
@@ -1488,7 +1489,7 @@
         <v>8.7164224410896942</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>22</v>
       </c>
@@ -1505,7 +1506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>22</v>
       </c>
@@ -1522,7 +1523,7 @@
         <v>7.5745505493882419</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>22</v>
       </c>
@@ -1539,7 +1540,7 @@
         <v>8.7081192002671077</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>22</v>
       </c>
@@ -1556,7 +1557,7 @@
         <v>8.6683062227867484</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>22</v>
       </c>
@@ -1573,7 +1574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>22</v>
       </c>
@@ -1590,7 +1591,7 @@
         <v>8.3711047078267224</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>25</v>
       </c>
@@ -1607,7 +1608,7 @@
         <v>8.1871312677259507</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>25</v>
       </c>
@@ -1624,7 +1625,7 @@
         <v>7.834637471548743</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>25</v>
       </c>
@@ -1641,7 +1642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>25</v>
       </c>
@@ -1658,7 +1659,7 @@
         <v>7.1895477474602121</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>25</v>
       </c>
@@ -1675,7 +1676,7 @@
         <v>8.3211185780394441</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>25</v>
       </c>
@@ -1692,7 +1693,7 @@
         <v>7.7246875247966642</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>25</v>
       </c>
@@ -1709,7 +1710,7 @@
         <v>7.9438290492761165</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>25</v>
       </c>
@@ -1726,7 +1727,7 @@
         <v>9.0557305603392173</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>25</v>
       </c>
@@ -1743,7 +1744,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>25</v>
       </c>
@@ -1760,7 +1761,7 @@
         <v>7.3173425999192094</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>25</v>
       </c>
@@ -1777,7 +1778,7 @@
         <v>7.7784475255210337</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>25</v>
       </c>
@@ -1794,7 +1795,7 @@
         <v>8.555675164430923</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>11</v>
       </c>
@@ -1811,7 +1812,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>11</v>
       </c>
@@ -1828,7 +1829,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>11</v>
       </c>
@@ -1845,7 +1846,7 @@
         <v>9.9082873968112128</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>11</v>
       </c>
@@ -1862,7 +1863,7 @@
         <v>9.5951632705470598</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>11</v>
       </c>
@@ -1879,7 +1880,7 @@
         <v>7.9070778741133312</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>11</v>
       </c>
@@ -1896,7 +1897,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>11</v>
       </c>
@@ -1913,7 +1914,7 @@
         <v>8.6902798693190064</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>11</v>
       </c>
@@ -1930,7 +1931,7 @@
         <v>7.8966627789513231</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>11</v>
       </c>
@@ -1947,7 +1948,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>11</v>
       </c>
@@ -1964,7 +1965,7 @@
         <v>7.0037696043742921</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>11</v>
       </c>
@@ -1981,7 +1982,7 @@
         <v>9.8694833556364721</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>11</v>
       </c>
@@ -1998,7 +1999,7 @@
         <v>7.31460090614988</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>8</v>
       </c>
@@ -2015,7 +2016,7 @@
         <v>4.1627242570574046</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>8</v>
       </c>
@@ -2032,7 +2033,7 @@
         <v>5.4064712652896914</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>8</v>
       </c>
@@ -2049,7 +2050,7 @@
         <v>5.5844943069811936</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>8</v>
       </c>
@@ -2066,7 +2067,7 @@
         <v>6.7441211318146834</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>8</v>
       </c>
@@ -2083,7 +2084,7 @@
         <v>4.8201349673318052</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>8</v>
       </c>
@@ -2100,7 +2101,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>8</v>
       </c>
@@ -2117,7 +2118,7 @@
         <v>7.8450372899315797</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>8</v>
       </c>
@@ -2134,7 +2135,7 @@
         <v>6.5562133199314827</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>8</v>
       </c>
@@ -2151,7 +2152,7 @@
         <v>5.6118916282004454</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>8</v>
       </c>
@@ -2168,7 +2169,7 @@
         <v>4.1870604839832515</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>8</v>
       </c>
@@ -2185,7 +2186,7 @@
         <v>4.8069955913927958</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>8</v>
       </c>
@@ -2202,7 +2203,7 @@
         <v>4.702158937613186</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>30</v>
       </c>
@@ -2219,7 +2220,7 @@
         <v>5.4458777901474074</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>30</v>
       </c>
@@ -2236,7 +2237,7 @@
         <v>5.6291090339227239</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>30</v>
       </c>
@@ -2253,7 +2254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>30</v>
       </c>
@@ -2270,7 +2271,7 @@
         <v>7.1321963587468638</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>30</v>
       </c>
@@ -2287,7 +2288,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>30</v>
       </c>
@@ -2304,7 +2305,7 @@
         <v>4.8214051487949972</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>30</v>
       </c>
@@ -2321,7 +2322,7 @@
         <v>4.6218074597143648</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>30</v>
       </c>
@@ -2338,7 +2339,7 @@
         <v>4.5479928850792897</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>30</v>
       </c>
@@ -2355,7 +2356,7 @@
         <v>4.7506231416755345</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>30</v>
       </c>
@@ -2372,7 +2373,7 @@
         <v>6.7764744195570428</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>30</v>
       </c>
@@ -2389,7 +2390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>30</v>
       </c>
@@ -2406,7 +2407,7 @@
         <v>6.5520812338215775</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>24</v>
       </c>
@@ -2423,7 +2424,7 @@
         <v>4.6627135450070423</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>24</v>
       </c>
@@ -2440,7 +2441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>24</v>
       </c>
@@ -2457,7 +2458,7 @@
         <v>5.6266655529385545</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>24</v>
       </c>
@@ -2474,7 +2475,7 @@
         <v>6.6065409406277169</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>24</v>
       </c>
@@ -2491,7 +2492,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>24</v>
       </c>
@@ -2508,7 +2509,7 @@
         <v>4.4147785028849658</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>24</v>
       </c>
@@ -2525,7 +2526,7 @@
         <v>5.1237013474829283</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>24</v>
       </c>
@@ -2542,7 +2543,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>24</v>
       </c>
@@ -2559,7 +2560,7 @@
         <v>5.5070130494490446</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>24</v>
       </c>
@@ -2576,7 +2577,7 @@
         <v>6.4438043127410589</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>24</v>
       </c>
@@ -2593,7 +2594,7 @@
         <v>6.0470066319242148</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>24</v>
       </c>
@@ -2610,7 +2611,7 @@
         <v>4.4332119011325499</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>17</v>
       </c>
@@ -2627,7 +2628,7 @@
         <v>7.4148828169392225</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>17</v>
       </c>
@@ -2644,7 +2645,7 @@
         <v>4.60656958711317</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>17</v>
       </c>
@@ -2661,7 +2662,7 @@
         <v>4.7882484900961941</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>17</v>
       </c>
@@ -2678,7 +2679,7 @@
         <v>7.991183141789171</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>17</v>
       </c>
@@ -2695,7 +2696,7 @@
         <v>4.2328071839252583</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>17</v>
       </c>
@@ -2712,7 +2713,7 @@
         <v>7.5588690572872066</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>17</v>
       </c>
@@ -2729,7 +2730,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>17</v>
       </c>
@@ -2746,7 +2747,7 @@
         <v>4.642374971278187</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>17</v>
       </c>
@@ -2763,7 +2764,7 @@
         <v>6.4414590277537407</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>17</v>
       </c>
@@ -2780,7 +2781,7 @@
         <v>5.9417298188336796</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>17</v>
       </c>
@@ -2797,7 +2798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>17</v>
       </c>
@@ -2814,7 +2815,7 @@
         <v>4.4504816784260406</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>23</v>
       </c>
@@ -2831,7 +2832,7 @@
         <v>6.4796043726102237</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>23</v>
       </c>
@@ -2848,7 +2849,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>23</v>
       </c>
@@ -2865,7 +2866,7 @@
         <v>6.6549546973440759</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>23</v>
       </c>
@@ -2882,7 +2883,7 @@
         <v>6.9963109415953673</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>23</v>
       </c>
@@ -2899,7 +2900,7 @@
         <v>6.7777506234634775</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>23</v>
       </c>
@@ -2916,7 +2917,7 @@
         <v>5.9696444444718217</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>23</v>
       </c>
@@ -2933,7 +2934,7 @@
         <v>5.8902059117106971</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>23</v>
       </c>
@@ -2950,7 +2951,7 @@
         <v>6.8004651135825087</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>23</v>
       </c>
@@ -2967,7 +2968,7 @@
         <v>5.5787217756267218</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>23</v>
       </c>
@@ -2984,7 +2985,7 @@
         <v>7.5676828209221414</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>23</v>
       </c>
@@ -3001,7 +3002,7 @@
         <v>4.8547566066794321</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>23</v>
       </c>
@@ -3018,7 +3019,7 @@
         <v>4.1527632682028575</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>14</v>
       </c>
@@ -3035,7 +3036,7 @@
         <v>4.8479065750094801</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>14</v>
       </c>
@@ -3052,7 +3053,7 @@
         <v>4.4435837018784881</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>14</v>
       </c>
@@ -3069,7 +3070,7 @@
         <v>6.1597240615346802</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>14</v>
       </c>
@@ -3086,7 +3087,7 @@
         <v>4.9431536877731954</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>14</v>
       </c>
@@ -3103,7 +3104,7 @@
         <v>4.6799012278287933</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>14</v>
       </c>
@@ -3120,7 +3121,7 @@
         <v>4.5444333162814656</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>14</v>
       </c>
@@ -3137,7 +3138,7 @@
         <v>6.3141594366504741</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>14</v>
       </c>
@@ -3154,7 +3155,7 @@
         <v>7.7370267264562838</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>14</v>
       </c>
@@ -3171,7 +3172,7 @@
         <v>4.5416996664457034</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>14</v>
       </c>
@@ -3188,7 +3189,7 @@
         <v>5.4435868348070304</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>14</v>
       </c>
@@ -3205,7 +3206,7 @@
         <v>4.6156892796765101</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>14</v>
       </c>
@@ -3222,7 +3223,7 @@
         <v>5.7102046324820304</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>18</v>
       </c>
@@ -3239,7 +3240,7 @@
         <v>6.2644049602885294</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>18</v>
       </c>
@@ -3256,7 +3257,7 @@
         <v>4.9945123391581401</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>18</v>
       </c>
@@ -3273,7 +3274,7 @@
         <v>5.26217021348989</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>18</v>
       </c>
@@ -3290,7 +3291,7 @@
         <v>7.3070851640519674</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>18</v>
       </c>
@@ -3307,7 +3308,7 @@
         <v>6.0871384473757182</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>18</v>
       </c>
@@ -3324,7 +3325,7 @@
         <v>6.8266063084833899</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>18</v>
       </c>
@@ -3341,7 +3342,7 @@
         <v>5.8576252159867579</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>18</v>
       </c>
@@ -3358,7 +3359,7 @@
         <v>6.1356699182941812</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>18</v>
       </c>
@@ -3375,7 +3376,7 @@
         <v>6.8720072572532214</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>18</v>
       </c>
@@ -3392,7 +3393,7 @@
         <v>4.3976524565000181</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>18</v>
       </c>
@@ -3409,7 +3410,7 @@
         <v>6.0367102127217596</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>18</v>
       </c>
@@ -3426,7 +3427,7 @@
         <v>6.3660882092382041</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>10</v>
       </c>
@@ -3443,7 +3444,7 @@
         <v>5.297843657473531</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>10</v>
       </c>
@@ -3460,7 +3461,7 @@
         <v>7.5573359545162919</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>10</v>
       </c>
@@ -3477,7 +3478,7 @@
         <v>7.7524456866920151</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>10</v>
       </c>
@@ -3494,7 +3495,7 @@
         <v>7.413478830229927</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>10</v>
       </c>
@@ -3511,7 +3512,7 @@
         <v>5.1718295690144185</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>10</v>
       </c>
@@ -3528,7 +3529,7 @@
         <v>6.9259666889007692</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>10</v>
       </c>
@@ -3545,7 +3546,7 @@
         <v>6.9791927826968951</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>10</v>
       </c>
@@ -3562,7 +3563,7 @@
         <v>4.1233555326082474</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>10</v>
       </c>
@@ -3579,7 +3580,7 @@
         <v>5.7041541620968914</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>10</v>
       </c>
@@ -3596,7 +3597,7 @@
         <v>5.7840188904011409</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>10</v>
       </c>
@@ -3613,7 +3614,7 @@
         <v>5.4034630502672876</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>10</v>
       </c>
@@ -3630,7 +3631,7 @@
         <v>7.6934169687069964</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>13</v>
       </c>
@@ -3647,7 +3648,7 @@
         <v>4.5585500937161489</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>13</v>
       </c>
@@ -3664,7 +3665,7 @@
         <v>6.9412532208596334</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>13</v>
       </c>
@@ -3681,7 +3682,7 @@
         <v>5.3724779263684797</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>13</v>
       </c>
@@ -3698,7 +3699,7 @@
         <v>4.6065080517583201</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>13</v>
       </c>
@@ -3715,7 +3716,7 @@
         <v>5.2925134410946377</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>13</v>
       </c>
@@ -3732,7 +3733,7 @@
         <v>5.4528986993806212</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>13</v>
       </c>
@@ -3749,7 +3750,7 @@
         <v>4.0514124649951864</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>13</v>
       </c>
@@ -3766,7 +3767,7 @@
         <v>7.9816640260833633</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>13</v>
       </c>
@@ -3783,7 +3784,7 @@
         <v>5.3105703337794097</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>13</v>
       </c>
@@ -3800,7 +3801,7 @@
         <v>7.8863325514947249</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>13</v>
       </c>
@@ -3817,7 +3818,7 @@
         <v>6.6923079709308837</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>13</v>
       </c>
@@ -3834,7 +3835,7 @@
         <v>7.6543984402703789</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>5</v>
       </c>
@@ -3851,7 +3852,7 @@
         <v>5.5496752969568384</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>5</v>
       </c>
@@ -3868,7 +3869,7 @@
         <v>4.6342311248891628</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>5</v>
       </c>
@@ -3885,7 +3886,7 @@
         <v>7.8846487341436955</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>5</v>
       </c>
@@ -3902,7 +3903,7 @@
         <v>5.6505148659144684</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>5</v>
       </c>
@@ -3919,7 +3920,7 @@
         <v>5.4515124187834276</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>5</v>
       </c>
@@ -3936,7 +3937,7 @@
         <v>7.2842671787324278</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>5</v>
       </c>
@@ -3953,7 +3954,7 @@
         <v>6.2967982837351277</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>5</v>
       </c>
@@ -3970,7 +3971,7 @@
         <v>5.8476722118852242</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>5</v>
       </c>
@@ -3987,7 +3988,7 @@
         <v>6.7130153540268154</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>5</v>
       </c>
@@ -4004,7 +4005,7 @@
         <v>6.1230937979550211</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>5</v>
       </c>
@@ -4021,7 +4022,7 @@
         <v>5.3741459053688212</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>5</v>
       </c>
@@ -4038,7 +4039,7 @@
         <v>4.5776073656312093</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>33</v>
       </c>
@@ -4055,7 +4056,7 @@
         <v>6.7445267910734392</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>33</v>
       </c>
@@ -4072,7 +4073,7 @@
         <v>5.4537392311602648</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>33</v>
       </c>
@@ -4089,7 +4090,7 @@
         <v>6.2477623482300224</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>33</v>
       </c>
@@ -4106,7 +4107,7 @@
         <v>4.5178660393037591</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>33</v>
       </c>
@@ -4123,7 +4124,7 @@
         <v>7.6177178198407116</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>33</v>
       </c>
@@ -4140,7 +4141,7 @@
         <v>6.0251407933661012</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>33</v>
       </c>
@@ -4157,7 +4158,7 @@
         <v>5.8317729408528729</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>33</v>
       </c>
@@ -4174,7 +4175,7 @@
         <v>4.1899725542096489</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>33</v>
       </c>
@@ -4191,7 +4192,7 @@
         <v>6.818157397947771</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>33</v>
       </c>
@@ -4208,7 +4209,7 @@
         <v>5.3695127231740978</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>33</v>
       </c>
@@ -4225,7 +4226,7 @@
         <v>7.9413827803174648</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>33</v>
       </c>
@@ -4242,7 +4243,7 @@
         <v>6.773161597518035</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>27</v>
       </c>
@@ -4259,7 +4260,7 @@
         <v>6.2182199115591024</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>27</v>
       </c>
@@ -4276,7 +4277,7 @@
         <v>5.4142658241386883</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>27</v>
       </c>
@@ -4293,7 +4294,7 @@
         <v>6.9919343572911412</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>27</v>
       </c>
@@ -4310,7 +4311,7 @@
         <v>6.6382251400359129</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>27</v>
       </c>
@@ -4327,7 +4328,7 @@
         <v>7.1829393647104069</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>27</v>
       </c>
@@ -4344,7 +4345,7 @@
         <v>5.5488019485602589</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>27</v>
       </c>
@@ -4361,7 +4362,7 @@
         <v>7.7892350001041457</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>27</v>
       </c>
@@ -4378,7 +4379,7 @@
         <v>4.2563108773142115</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>27</v>
       </c>
@@ -4395,7 +4396,7 @@
         <v>4.8929463028666174</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>27</v>
       </c>
@@ -4412,7 +4413,7 @@
         <v>4.0054898970454369</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>27</v>
       </c>
@@ -4429,7 +4430,7 @@
         <v>4.9598087017315722</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>27</v>
       </c>
@@ -4446,7 +4447,7 @@
         <v>7.6940779472921008</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>29</v>
       </c>
@@ -4463,7 +4464,7 @@
         <v>6.1254900375386798</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>29</v>
       </c>
@@ -4480,7 +4481,7 @@
         <v>5.6866205338614026</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>29</v>
       </c>
@@ -4497,7 +4498,7 @@
         <v>7.4095623419987362</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>29</v>
       </c>
@@ -4514,7 +4515,7 @@
         <v>6.9185936074612346</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>29</v>
       </c>
@@ -4531,7 +4532,7 @@
         <v>4.5865863367367243</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>29</v>
       </c>
@@ -4548,7 +4549,7 @@
         <v>6.7772791134086292</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>29</v>
       </c>
@@ -4565,7 +4566,7 @@
         <v>7.3081327999811112</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>29</v>
       </c>
@@ -4582,7 +4583,7 @@
         <v>5.9896817591346325</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>29</v>
       </c>
@@ -4599,7 +4600,7 @@
         <v>4.6022108389671832</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>29</v>
       </c>
@@ -4616,7 +4617,7 @@
         <v>5.0613311968640318</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>29</v>
       </c>
@@ -4633,7 +4634,7 @@
         <v>5.9725355273170813</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>29</v>
       </c>
@@ -4650,7 +4651,7 @@
         <v>4.2505944523320531</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>16</v>
       </c>
@@ -4667,7 +4668,7 @@
         <v>6.9760029240891965</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>16</v>
       </c>
@@ -4684,7 +4685,7 @@
         <v>7.8066400254979849</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>16</v>
       </c>
@@ -4701,7 +4702,7 @@
         <v>5.8149068242007091</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>16</v>
       </c>
@@ -4718,7 +4719,7 @@
         <v>4.1089307739099983</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>16</v>
       </c>
@@ -4735,7 +4736,7 @@
         <v>4.5546920589564701</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>16</v>
       </c>
@@ -4752,7 +4753,7 @@
         <v>6.6601957103196492</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>16</v>
       </c>
@@ -4769,7 +4770,7 @@
         <v>5.1797512548798315</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>16</v>
       </c>
@@ -4786,7 +4787,7 @@
         <v>5.9296660957623768</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>16</v>
       </c>
@@ -4803,7 +4804,7 @@
         <v>7.7073315877038988</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>16</v>
       </c>
@@ -4820,7 +4821,7 @@
         <v>6.5544800115994519</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>16</v>
       </c>
@@ -4837,7 +4838,7 @@
         <v>4.169448667806801</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>16</v>
       </c>
@@ -4854,7 +4855,7 @@
         <v>7.6004513139258272</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>26</v>
       </c>
@@ -4871,7 +4872,7 @@
         <v>5.2907737756956346</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>26</v>
       </c>
@@ -4888,7 +4889,7 @@
         <v>7.4927556975795264</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>26</v>
       </c>
@@ -4905,7 +4906,7 @@
         <v>5.1189609425239988</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>26</v>
       </c>
@@ -4922,7 +4923,7 @@
         <v>6.7806614502732288</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>26</v>
       </c>
@@ -4939,7 +4940,7 @@
         <v>4.3495864892325109</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>26</v>
       </c>
@@ -4956,7 +4957,7 @@
         <v>4.4446049258748301</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>26</v>
       </c>
@@ -4973,7 +4974,7 @@
         <v>5.4831210369225412</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>26</v>
       </c>
@@ -4990,7 +4991,7 @@
         <v>6.8603196930071668</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>26</v>
       </c>
@@ -5007,7 +5008,7 @@
         <v>5.9699865013231044</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>26</v>
       </c>
@@ -5024,7 +5025,7 @@
         <v>5.1193851894487059</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>26</v>
       </c>
@@ -5041,7 +5042,7 @@
         <v>5.6996494654242555</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>26</v>
       </c>
@@ -5058,7 +5059,7 @@
         <v>7.5563371065218474</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>19</v>
       </c>
@@ -5075,7 +5076,7 @@
         <v>5.9872142458105868</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>19</v>
       </c>
@@ -5092,7 +5093,7 @@
         <v>7.5674482911193399</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>19</v>
       </c>
@@ -5109,7 +5110,7 @@
         <v>6.0815019116521309</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>19</v>
       </c>
@@ -5126,7 +5127,7 @@
         <v>5.3435167821388543</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>19</v>
       </c>
@@ -5143,7 +5144,7 @@
         <v>4.877299140032525</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>19</v>
       </c>
@@ -5160,7 +5161,7 @@
         <v>7.4678252591139334</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>19</v>
       </c>
@@ -5177,7 +5178,7 @@
         <v>7.6715266366950035</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>19</v>
       </c>
@@ -5194,7 +5195,7 @@
         <v>6.9933281344158233</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>19</v>
       </c>
@@ -5211,7 +5212,7 @@
         <v>4.4732152739581217</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>19</v>
       </c>
@@ -5228,7 +5229,7 @@
         <v>7.7992966487965703</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>19</v>
       </c>
@@ -5245,7 +5246,7 @@
         <v>7.1863730943000785</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>19</v>
       </c>
@@ -5262,7 +5263,7 @@
         <v>6.5305570455328628</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>34</v>
       </c>
@@ -5279,7 +5280,7 @@
         <v>7.2329457362615033</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>34</v>
       </c>
@@ -5296,7 +5297,7 @@
         <v>7.1811219980209078</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>34</v>
       </c>
@@ -5313,7 +5314,7 @@
         <v>5.049803009865883</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>34</v>
       </c>
@@ -5330,7 +5331,7 @@
         <v>4.0755760888862911</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>34</v>
       </c>
@@ -5347,7 +5348,7 @@
         <v>5.2171381991353236</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>34</v>
       </c>
@@ -5364,7 +5365,7 @@
         <v>6.1415552671394202</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>34</v>
       </c>
@@ -5381,7 +5382,7 @@
         <v>5.3049381158336386</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>34</v>
       </c>
@@ -5398,7 +5399,7 @@
         <v>6.8962550037878962</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>34</v>
       </c>
@@ -5415,7 +5416,7 @@
         <v>6.4013435970825254</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>34</v>
       </c>
@@ -5432,7 +5433,7 @@
         <v>7.2127523703271823</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>34</v>
       </c>
@@ -5449,7 +5450,7 @@
         <v>5.669705980081293</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>34</v>
       </c>
@@ -5466,7 +5467,7 @@
         <v>6.4303618728960021</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>20</v>
       </c>
@@ -5483,7 +5484,7 @@
         <v>6.4657343281667687</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>20</v>
       </c>
@@ -5500,7 +5501,7 @@
         <v>4.0397426917918171</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>20</v>
       </c>
@@ -5517,7 +5518,7 @@
         <v>5.8026702693098988</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>20</v>
       </c>
@@ -5534,7 +5535,7 @@
         <v>7.4486409481991824</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>20</v>
       </c>
@@ -5551,7 +5552,7 @@
         <v>6.8109305460686889</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>20</v>
       </c>
@@ -5568,7 +5569,7 @@
         <v>4.9384197703140629</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>20</v>
       </c>
@@ -5585,7 +5586,7 @@
         <v>7.5943346417469062</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>20</v>
       </c>
@@ -5602,7 +5603,7 @@
         <v>6.5698136523658839</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>20</v>
       </c>
@@ -5619,7 +5620,7 @@
         <v>5.5368372158859476</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>20</v>
       </c>
@@ -5636,7 +5637,7 @@
         <v>7.7368164398647723</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>20</v>
       </c>
@@ -5653,7 +5654,7 @@
         <v>4.6614246253582508</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>20</v>
       </c>
@@ -5670,7 +5671,7 @@
         <v>6.8076200361896611</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>15</v>
       </c>
@@ -5687,7 +5688,7 @@
         <v>5.2359241594681087</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>15</v>
       </c>
@@ -5704,7 +5705,7 @@
         <v>6.5588712524078749</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>15</v>
       </c>
@@ -5721,7 +5722,7 @@
         <v>4.9825173061418475</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>15</v>
       </c>
@@ -5738,7 +5739,7 @@
         <v>7.7919586038507074</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>15</v>
       </c>
@@ -5755,7 +5756,7 @@
         <v>7.6767855385346282</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>15</v>
       </c>
@@ -5772,7 +5773,7 @@
         <v>7.3734592328886199</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>15</v>
       </c>
@@ -5789,7 +5790,7 @@
         <v>4.4113780108711218</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>15</v>
       </c>
@@ -5806,7 +5807,7 @@
         <v>4.6405246586867168</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>15</v>
       </c>
@@ -5823,7 +5824,7 @@
         <v>6.0569998566636158</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>15</v>
       </c>
@@ -5840,7 +5841,7 @@
         <v>7.3668823581298088</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>15</v>
       </c>
@@ -5857,7 +5858,7 @@
         <v>6.0887816428429238</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
         <v>15</v>
       </c>
@@ -5874,7 +5875,7 @@
         <v>7.5153442349352417</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>28</v>
       </c>
@@ -5891,7 +5892,7 @@
         <v>6.1490990736036144</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
         <v>28</v>
       </c>
@@ -5908,7 +5909,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
         <v>28</v>
       </c>
@@ -5925,7 +5926,7 @@
         <v>5.4469381559588861</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
         <v>28</v>
       </c>
@@ -5942,7 +5943,7 @@
         <v>5.0968143104186616</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
         <v>28</v>
       </c>
@@ -5959,7 +5960,7 @@
         <v>6.5603957994642901</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
         <v>28</v>
       </c>
@@ -5976,7 +5977,7 @@
         <v>7.7813411306176876</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
         <v>28</v>
       </c>
@@ -5993,7 +5994,7 @@
         <v>5.7390083383511517</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
         <v>28</v>
       </c>
@@ -6010,7 +6011,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>28</v>
       </c>
@@ -6027,7 +6028,7 @@
         <v>4.316811200095974</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
         <v>28</v>
       </c>
@@ -6044,7 +6045,7 @@
         <v>6.7461640142328223</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>28</v>
       </c>
@@ -6061,7 +6062,7 @@
         <v>4.0962733651629737</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
         <v>28</v>
       </c>
@@ -6078,7 +6079,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
         <v>32</v>
       </c>
@@ -6095,7 +6096,7 @@
         <v>5.7550742276003195</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
         <v>32</v>
       </c>
@@ -6112,7 +6113,7 @@
         <v>4.2920657804726234</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>32</v>
       </c>
@@ -6129,7 +6130,7 @@
         <v>9.2097017906064362</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
         <v>32</v>
       </c>
@@ -6146,7 +6147,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
         <v>32</v>
       </c>
@@ -6163,7 +6164,7 @@
         <v>0.84725770546971035</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
         <v>32</v>
       </c>
@@ -6180,7 +6181,7 @@
         <v>3.8370580914126466</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
         <v>32</v>
       </c>
@@ -6197,7 +6198,7 @@
         <v>2.3077452395109086</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
         <v>32</v>
       </c>
@@ -6214,7 +6215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
         <v>32</v>
       </c>
@@ -6231,7 +6232,7 @@
         <v>7.6980764604877869</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
         <v>32</v>
       </c>
@@ -6248,7 +6249,7 @@
         <v>3.9093663223298778</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
         <v>32</v>
       </c>
@@ -6265,7 +6266,7 @@
         <v>3.2369903778075071</v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>32</v>
       </c>
@@ -6282,7 +6283,7 @@
         <v>4.6705226641994795</v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>7</v>
       </c>
@@ -6299,7 +6300,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
         <v>7</v>
       </c>
@@ -6316,7 +6317,7 @@
         <v>3.5001370103741234</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>7</v>
       </c>
@@ -6333,7 +6334,7 @@
         <v>8.8662639158421044</v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
         <v>7</v>
       </c>
@@ -6350,7 +6351,7 @@
         <v>0.81465114820975071</v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
         <v>7</v>
       </c>
@@ -6367,7 +6368,7 @@
         <v>5.0033519655164529</v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
         <v>7</v>
       </c>
@@ -6384,7 +6385,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
         <v>7</v>
       </c>
@@ -6401,7 +6402,7 @@
         <v>8.0541214307916604</v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
         <v>7</v>
       </c>
@@ -6418,7 +6419,7 @@
         <v>1.6183762712411562</v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
         <v>7</v>
       </c>
@@ -6435,7 +6436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
         <v>7</v>
       </c>
@@ -6452,7 +6453,7 @@
         <v>0.86310888238539163</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>7</v>
       </c>
@@ -6469,7 +6470,7 @@
         <v>9.8373457547643781</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
         <v>7</v>
       </c>
@@ -6486,7 +6487,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>12</v>
       </c>
@@ -6503,7 +6504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
         <v>12</v>
       </c>
@@ -6520,7 +6521,7 @@
         <v>1.8650554193306854</v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
         <v>12</v>
       </c>
@@ -6537,7 +6538,7 @@
         <v>6.8637914551266439</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
         <v>12</v>
       </c>
@@ -6554,7 +6555,7 @@
         <v>5.9210697934249756</v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
         <v>12</v>
       </c>
@@ -6571,7 +6572,7 @@
         <v>1.2784866750582395</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
         <v>12</v>
       </c>
@@ -6588,7 +6589,7 @@
         <v>6.7686176852659896</v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
         <v>12</v>
       </c>
@@ -6605,7 +6606,7 @@
         <v>8.9922269914382067</v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
         <v>12</v>
       </c>
@@ -6622,7 +6623,7 @@
         <v>1.6032283154539524</v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
         <v>12</v>
       </c>
@@ -6639,7 +6640,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
         <v>12</v>
       </c>
@@ -6656,7 +6657,7 @@
         <v>8.446391646491989</v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
         <v>12</v>
       </c>
@@ -6673,7 +6674,7 @@
         <v>3.7767343888597313</v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
         <v>12</v>
       </c>
@@ -6690,18 +6691,18 @@
         <v>0.30101836548213567</v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C362" s="4"/>
       <c r="D362" s="4"/>
       <c r="E362" s="4"/>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C363" s="4"/>
       <c r="D363" s="4"/>
       <c r="E363" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E31" xr:uid="{BDD9A485-9C40-4281-B8A0-78879B8E3C17}">
+  <autoFilter ref="A1:E31">
     <sortState ref="A2:E361">
       <sortCondition ref="A1:A31"/>
     </sortState>
@@ -6712,18 +6713,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A817D5D9-A97B-4002-BCCC-EE0C30B8468A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6731,7 +6732,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -6739,7 +6740,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -6747,7 +6748,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -6755,7 +6756,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -6763,7 +6764,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -6771,7 +6772,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -6779,7 +6780,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -6787,7 +6788,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -6795,7 +6796,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -6803,7 +6804,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -6811,7 +6812,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -6819,7 +6820,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -6827,7 +6828,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -6835,7 +6836,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -6843,7 +6844,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -6851,7 +6852,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -6859,7 +6860,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -6867,7 +6868,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
@@ -6875,7 +6876,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>27</v>
       </c>
@@ -6883,7 +6884,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
@@ -6891,7 +6892,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -6899,7 +6900,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -6907,7 +6908,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
@@ -6915,7 +6916,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -6923,7 +6924,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>20</v>
       </c>
@@ -6931,7 +6932,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
@@ -6939,7 +6940,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -6947,7 +6948,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -6955,7 +6956,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -6963,7 +6964,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>